<commit_message>
New Domains added, fixed bug where when only level is selected a sheet can not be created.
</commit_message>
<xml_diff>
--- a/lib/classes/cleric/DivineDomains.xlsx
+++ b/lib/classes/cleric/DivineDomains.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="41">
   <si>
     <t>Ambition Domain</t>
   </si>
@@ -19,18 +19,87 @@
     <t>Arcana Domain</t>
   </si>
   <si>
+    <t>Beauty Domain</t>
+  </si>
+  <si>
+    <t>Blood Domain</t>
+  </si>
+  <si>
+    <t>City Domain</t>
+  </si>
+  <si>
+    <t>Death Domain</t>
+  </si>
+  <si>
+    <t>Fate Domain</t>
+  </si>
+  <si>
+    <t>Forge Domain</t>
+  </si>
+  <si>
+    <t>Grave Domain</t>
+  </si>
+  <si>
+    <t>Knowledge Domain</t>
+  </si>
+  <si>
+    <t>Life Domain</t>
+  </si>
+  <si>
     <t>None</t>
   </si>
   <si>
+    <t>Heavy Armor</t>
+  </si>
+  <si>
+    <t>Martial Weapons</t>
+  </si>
+  <si>
+    <t>Sidearms=Vehicles (Land)</t>
+  </si>
+  <si>
+    <t>Smith’s tools</t>
+  </si>
+  <si>
     <t>Arcana</t>
   </si>
   <si>
+    <t>Arcana=Religion</t>
+  </si>
+  <si>
     <t>true=classes/cleric/domains/BonusSpellsAmbitionDomain.xlsx</t>
   </si>
   <si>
     <t>true=classes/cleric/domains/BonusSpellsArcaneDomain.xlsx</t>
   </si>
   <si>
+    <t>true=classes/cleric/domains/BonusSpellsBeautyDomain.xlsx</t>
+  </si>
+  <si>
+    <t>true=classes/cleric/domains/BonusSpellsBloodDomain.xlsx</t>
+  </si>
+  <si>
+    <t>true=classes/cleric/domains/BonusSpellsCityDomain.xlsx</t>
+  </si>
+  <si>
+    <t>true=classes/cleric/domains/BonusSpellsDeathDomain.xlsx</t>
+  </si>
+  <si>
+    <t>true=classes/cleric/domains/BonusSpellsFateDomain.xlsx</t>
+  </si>
+  <si>
+    <t>true=classes/cleric/domains/BonusSpellsForgeDomain.xlsx</t>
+  </si>
+  <si>
+    <t>true=classes/cleric/domains/BonusSpellsGraveDomain.xlsx</t>
+  </si>
+  <si>
+    <t>true=classes/cleric/domains/BonusSpellsKnowledgeDomain.xlsx</t>
+  </si>
+  <si>
+    <t>true=classes/cleric/domains/BonusSpellsLifeDomain.xlsx</t>
+  </si>
+  <si>
     <t>false=</t>
   </si>
   <si>
@@ -38,6 +107,33 @@
   </si>
   <si>
     <t>2/Channel Divinity: Arcane Abjuration=6/Spell Breaker=8/Potent Spellcasting</t>
+  </si>
+  <si>
+    <t>1/Beauty's Refuge=2/Rebuke the Defiler=2/Channel Divinity: Beauty's Truce=6/Superior Refuge=8/Potent Cantrip=17/Soul of Beauty</t>
+  </si>
+  <si>
+    <t>1/Bloodletting Focus=2/Channel Divinity: Blood Puppet=6/Channel Divinity: Crimson Bond=8/Sanguine Recall=17/Vascular Corruption Aura</t>
+  </si>
+  <si>
+    <t>1/Heart of the City=2/Channel Divinity: Spirits of the City=6/Block Watch=8/Divine Strike=17/Express Transit</t>
+  </si>
+  <si>
+    <t>2/Channel Divinity: Touch of Death=6/Inescapable Destruction=8/Divine Strike=17/Improved Reaper</t>
+  </si>
+  <si>
+    <t>1/Omens and Portents=1/Ties That Bind=2/Channel Divinity: Strands of Fate=6/Insightful Striking=8/Potent Spellcasting=17/Visions of the Future</t>
+  </si>
+  <si>
+    <t>1/Blessing of the Forge=2/Channel Divinity: Artisan's Blessing=6/Soul of the Forge (Fire Resistance)=8/Divine Strike=17/Saint of Forge and Fire (Fire Immunity)</t>
+  </si>
+  <si>
+    <t>1/Circle of Mortality=1/Eyes of the Grave=2/Channel Divinity: Path to the Grave=6/Sentinel at Death's Door=8/Potent Spellcasting=17/Keeper of Souls</t>
+  </si>
+  <si>
+    <t>2/Channel Divinity: Knowledge of the Ages=6/Channel Divinity: Read Thoughts=8/Potent Spellcasting=17/Visions of the Past</t>
+  </si>
+  <si>
+    <t>1/Disciple of Life=2/Channel Divinity: Preserve Life=6/Blessed Healer=8/Divine Strike=17/Supreme Healing</t>
   </si>
 </sst>
 </file>
@@ -301,61 +397,277 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>2</v>
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>2</v>
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>3</v>
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>19</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>29</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All cleric domains added.
</commit_message>
<xml_diff>
--- a/lib/classes/cleric/DivineDomains.xlsx
+++ b/lib/classes/cleric/DivineDomains.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="84">
   <si>
     <t>Ambition Domain</t>
   </si>
@@ -46,6 +46,45 @@
     <t>Life Domain</t>
   </si>
   <si>
+    <t>Mind Domain</t>
+  </si>
+  <si>
+    <t>Nature Domain</t>
+  </si>
+  <si>
+    <t>Order Domain</t>
+  </si>
+  <si>
+    <t>Peace Domain</t>
+  </si>
+  <si>
+    <t>Protection Domain</t>
+  </si>
+  <si>
+    <t>Solidarity Domain</t>
+  </si>
+  <si>
+    <t>Strength Domain</t>
+  </si>
+  <si>
+    <t>Tempest Domain</t>
+  </si>
+  <si>
+    <t>Trickery Domain</t>
+  </si>
+  <si>
+    <t>Twilight Domain</t>
+  </si>
+  <si>
+    <t>Unity Domain</t>
+  </si>
+  <si>
+    <t>War Domain</t>
+  </si>
+  <si>
+    <t>Zeal Domain</t>
+  </si>
+  <si>
     <t>None</t>
   </si>
   <si>
@@ -64,7 +103,19 @@
     <t>Arcana</t>
   </si>
   <si>
-    <t>Arcana=Religion</t>
+    <t>Arcana/History/Nature/Religion=Arcana/History/Nature/Religion</t>
+  </si>
+  <si>
+    <t>Animal Handling/Nature/Survival</t>
+  </si>
+  <si>
+    <t>Intimidation/Persuasion</t>
+  </si>
+  <si>
+    <t>Insight/Performance/Persuasion</t>
+  </si>
+  <si>
+    <t>Animal Handling/Athletics/Nature/Survival</t>
   </si>
   <si>
     <t>true=classes/cleric/domains/BonusSpellsAmbitionDomain.xlsx</t>
@@ -100,6 +151,45 @@
     <t>true=classes/cleric/domains/BonusSpellsLifeDomain.xlsx</t>
   </si>
   <si>
+    <t>true=classes/cleric/domains/BonusSpellsMindDomain.xlsx</t>
+  </si>
+  <si>
+    <t>true=classes/cleric/domains/BonusSpellsNatureDomain.xlsx</t>
+  </si>
+  <si>
+    <t>true=classes/cleric/domains/BonusSpellsOrderDomain.xlsx</t>
+  </si>
+  <si>
+    <t>true=classes/cleric/domains/BonusSpellsPeaceDomain.xlsx</t>
+  </si>
+  <si>
+    <t>true=classes/cleric/domains/BonusSpellsProtectionDomain.xlsx</t>
+  </si>
+  <si>
+    <t>true=classes/cleric/domains/BonusSpellsSolidarityDomain.xlsx</t>
+  </si>
+  <si>
+    <t>true=classes/cleric/domains/BonusSpellsStrengthDomain.xlsx</t>
+  </si>
+  <si>
+    <t>true=classes/cleric/domains/BonusSpellsTempestDomain.xlsx</t>
+  </si>
+  <si>
+    <t>true=classes/cleric/domains/BonusSpellsTrickeryDomain.xlsx</t>
+  </si>
+  <si>
+    <t>true=classes/cleric/domains/BonusSpellsTwilightDomain.xlsx</t>
+  </si>
+  <si>
+    <t>true=classes/cleric/domains/BonusSpellsUnityDomain.xlsx</t>
+  </si>
+  <si>
+    <t>true=classes/cleric/domains/BonusSpellsWarDomain.xlsx</t>
+  </si>
+  <si>
+    <t>true=classes/cleric/domains/BonusSpellsZealDomain.xlsx</t>
+  </si>
+  <si>
     <t>false=</t>
   </si>
   <si>
@@ -134,6 +224,45 @@
   </si>
   <si>
     <t>1/Disciple of Life=2/Channel Divinity: Preserve Life=6/Blessed Healer=8/Divine Strike=17/Supreme Healing</t>
+  </si>
+  <si>
+    <t>1/Flash of Insight=1/Psychic Force=2/Channel Divinity: Psychic Feedback=6/Gestalt Anchor=8/Potent Spellcasting=17/Bend Reality</t>
+  </si>
+  <si>
+    <t>2/Channel Divinity: Charm Animals and Plants=6/Dampen Elements=8/Divine Strike=17/Master of Nature</t>
+  </si>
+  <si>
+    <t>1/Voice of Authority=2/Channel Divinity: Order's Demand=6/Embodiment of the Law=8/Divine Strike=17/Order's Wrath</t>
+  </si>
+  <si>
+    <t>1/Emboldening Bond=2/Channel Divinity: Balm of Peace=6/Protective Bond=8/Potent Spellcasting=17/Expansive Bond</t>
+  </si>
+  <si>
+    <t>1/Shield of the Faithful=2/Channel Divinity: Radiant Defense=6/Blessed Healer=8/Divine Strike=17/Indomitable Defense</t>
+  </si>
+  <si>
+    <t>1/Solidarity's Action=2/Channel Divinity: Preserve Life=6/Channel Divinity: Oketra's Blessing=8/Divine Strike=17/Supreme Healing</t>
+  </si>
+  <si>
+    <t>2/Channel Divinity: Feat of Strength=6/Channel Divinity: Rhonas' Blessing=8/Divine Strike=17/Avatar of Battle</t>
+  </si>
+  <si>
+    <t>1/Wrath of the Storm=2/Channel Divinity: Destructive Wrath=6/Thunderous Strike=8/Divine Strike=17/Stormborn</t>
+  </si>
+  <si>
+    <t>1/Blessing of the Trickster=2/Channel Divinity: Invoke Duplicity=6/Channel Divinity: Cloak of Shadows=8/Divine Strike=17/Improved Duplicity</t>
+  </si>
+  <si>
+    <t>1/Eyes of Night (Darkvision 300 ft)=1/Vigilant Blessing=2/Channel Divinity: Twilight Sanctuary=6/Steps of Night=8/Divine Strike=17/Twilight Shroud</t>
+  </si>
+  <si>
+    <t>1/Emboldening Bond=2/Channel Divinity: Shared Burden=6/Protective Bond=8/Potent Spellcasting=17/Enduring Unity</t>
+  </si>
+  <si>
+    <t>1/War Priest=2/Channel Divinity: Guided Strike=6/Channel Divinity: War God's Blessing=8/Divine Strike=17/Avatar of Battle</t>
+  </si>
+  <si>
+    <t>1/Priest of Zeal=2/Channel Divinity: Consuming Fervor=6/Resounding Strike=8/Divine Strike=17/Blaze of Glory</t>
   </si>
 </sst>
 </file>
@@ -424,250 +553,562 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>12</v>
+        <v>25</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>29</v>
+        <v>59</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>40</v>
+        <v>70</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bonus languages can now be granted by a class's archetype
</commit_message>
<xml_diff>
--- a/lib/classes/cleric/DivineDomains.xlsx
+++ b/lib/classes/cleric/DivineDomains.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="84">
   <si>
     <t>Ambition Domain</t>
   </si>
@@ -891,223 +891,297 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>56</v>
+        <v>24</v>
       </c>
       <c r="W6" s="1" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="X6" s="1" t="s">
-        <v>58</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="V7" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="W7" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="X7" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="K9" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="L9" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="M9" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="N9" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="O9" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="P8" s="1" t="s">
+      <c r="P9" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="Q9" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="R8" s="1" t="s">
+      <c r="R9" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="S8" s="1" t="s">
+      <c r="S9" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="T8" s="1" t="s">
+      <c r="T9" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="U8" s="1" t="s">
+      <c r="U9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="V8" s="1" t="s">
+      <c r="V9" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="W8" s="1" t="s">
+      <c r="W9" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="X8" s="1" t="s">
+      <c r="X9" s="1" t="s">
         <v>83</v>
       </c>
     </row>

</xml_diff>